<commit_message>
Added a ton of stuff
</commit_message>
<xml_diff>
--- a/Manual Test Case.xlsx
+++ b/Manual Test Case.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="228">
   <si>
     <t>TC16</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>TC1</t>
-  </si>
-  <si>
-    <t>TC2</t>
   </si>
   <si>
     <t>TC3</t>
@@ -229,32 +226,6 @@
     <t>TC22</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Check value of Carrier column if Set role </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>CanSeeCarrierNamer = False</t>
-    </r>
-  </si>
-  <si>
-    <t>See Carrier column: value of it is Carriercode1,Carriercode2……</t>
-  </si>
-  <si>
-    <t>See Carrier column: value of it is Carriername Carriercode1, Carriercode2…..) with site is MPLS
-With site is DIA: carrier column show value CarrierName</t>
-  </si>
-  <si>
-    <t>See Carrier column: value of it is Carriercode1,carriercode2…… with site is MPLS
-With site is DIA then show at the Carrier column to be "-"</t>
-  </si>
-  <si>
     <t>TC23</t>
   </si>
   <si>
@@ -288,32 +259,6 @@
     <t>TC33</t>
   </si>
   <si>
-    <t xml:space="preserve">                                                             Check value of Carrier column at the ClassicDIA Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See Carrier column: value of it is Carriername (Carriercode1,Carriercode2…..) </t>
-  </si>
-  <si>
-    <t>With Mode classic is fail
-ClassicDIA : Ok</t>
-  </si>
-  <si>
-    <t>With Mode classic ,
-ClassicDIA : Ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check value of TOTAL (A+P+CoS) Client Price NRC column </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check value of TOTAL (A+P+CoS) Client Price MRC column </t>
-  </si>
-  <si>
-    <t>TOTAL (A+P+CoS) Client Price NRC =Access Client Price NRC +Port Client Price NRC +CoS Voice Client Price NRC +CoS Voice Client Price NRC+CoS Premium (H) Client Price NRC+ CoS Premium (M) Client Price NRC+ CoS Premium (N) Client Price NRC+COS Best Effort Client Price NRC</t>
-  </si>
-  <si>
-    <t>TOTAL (A+P+CoS) Client Price MRC =Access Client Price MRC +Port Client Price MRC +CoS Voice Client Price MRC +CoS Voice Client Price MRC+CoS Premium (H) Client Price MRC+ CoS Premium (M) Client Price MRC+ CoS Premium (N) Client Price MRC+COS Best Effort Client Price MRC</t>
-  </si>
-  <si>
     <t>TC34</t>
   </si>
   <si>
@@ -323,54 +268,9 @@
     <t>TC36</t>
   </si>
   <si>
-    <t>7. Check value of TOTAL (A+P+CoS) Client Price NRC/MRC column at the Current, Classic, Expert Mode</t>
-  </si>
-  <si>
     <t>CR100 - Export to excel</t>
   </si>
   <si>
-    <t>1: Go to the system TestProEngine Classic Mode
-2: Create quote and submit for it
-3: Go to Maintenance User set role CanSeeCarrierName = True
-4: Open the quote
-5: Click [Export all Carriers] at Quick Links</t>
-  </si>
-  <si>
-    <t>1: Go to the system TestProEngine Classic Mode
-2: Create quote and submit for it
-3: Go to Maintenance User set role CanSeeCarrierName = False
-4: Open the quote
-5: Click [Export all Carriers] at Quick Links</t>
-  </si>
-  <si>
-    <t>1: Go to the system TestProEngine Classic Mode
-2: Create quote MPLS, DIA and submit for them
-3: Go to Maintenance User set role CanSeeCarrierName = True
-4: Open the quote
-5: Click [Export all Carriers] at Quick Links</t>
-  </si>
-  <si>
-    <t>1: Go to the system TestProEngine Classic Mode
-2: Create quote MPLS, DIA and submit for them
-3: Go to Maintenance User set role CanSeeCarrierName = False
-4: Open the quote
-5: Click [Export all Carriers] at Quick Links</t>
-  </si>
-  <si>
-    <t>1: Go to the system TestProEngine Classic Mode
-2: Create quote MPLS, DIA and submit for them
-3: Open the quote
-4: Click [Export all Carriers] at Quick Links
-5: See value of TOTAL (A+P+CoS) Client Price NRC</t>
-  </si>
-  <si>
-    <t>1: Go to the system TestProEngine Classic Mode
-2: Create quote MPLS, DIA and submit for them
-3: Open the quote
-4: Click [Export all Carriers] at Quick Links
-5: See value of TOTAL (A+P+CoS) Client Price MRC</t>
-  </si>
-  <si>
     <t>Sample ProjectACME Vacumm Cleaner &amp; Anvil Co. Feedback Form</t>
   </si>
   <si>
@@ -386,194 +286,581 @@
     <t>Site loads in Chrome, Safari, and FireFox</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
-    <t>Page anayltics event tracking works</t>
-  </si>
-  <si>
-    <t>Vertically centered within header. 15px from left edge.</t>
-  </si>
-  <si>
-    <t>21 px / Arial / italic. Horizontally centered inside the header, below the company name.</t>
-  </si>
-  <si>
-    <t>30 px / Arial. Horizontally centered inside the header, above the company moto.</t>
-  </si>
-  <si>
-    <t>21 px / Arial. Hover over turns the text yellow.</t>
-  </si>
-  <si>
     <t>Company logo</t>
   </si>
   <si>
-    <t>Company moto</t>
-  </si>
-  <si>
     <t>Company name</t>
   </si>
   <si>
-    <t>Mailing link style and hover</t>
-  </si>
-  <si>
-    <t>Mailing link click</t>
-  </si>
-  <si>
     <t>MANUAL TEST CASE</t>
   </si>
   <si>
     <t>Signup newsletter popup style</t>
   </si>
   <si>
-    <t>1. Sign Up for Out Newsletter: 18 px / Arial. Horizontally centered within the pop-up
-2. Email Address: Ghost Text: “Email Address”. Horizontally centered within the pop-up
-3. I certify that I am 18 years of age or older: 18px/ Arial. Horizontally centered within the pop-up.
+    <t>Email Validation: format</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I certify that I am 18 years of age or older has to be ticked</t>
+  </si>
+  <si>
+    <t>Signup with valid credentials</t>
+  </si>
+  <si>
+    <t>How did you hear about ACME VC&amp;A Co.? Style</t>
+  </si>
+  <si>
+    <t>How did you hear about ACME VC&amp;A Co.? Buttons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only one should be able to be selected. </t>
+  </si>
+  <si>
+    <t>How did you hear about ACME VC&amp;A Co.? Other Field</t>
+  </si>
+  <si>
+    <t>Should not be able to submit</t>
+  </si>
+  <si>
+    <t>How did you hear about ACME VC&amp;A Co.? Other Field passing</t>
+  </si>
+  <si>
+    <t>Should be able to submit</t>
+  </si>
+  <si>
+    <t>Rate your overall experience (1 - Very Poor, 5 - Very Good): Styling</t>
+  </si>
+  <si>
+    <t>Only one option can be selected</t>
+  </si>
+  <si>
+    <t>Rate your overall experience (1 - Very Poor, 5 - Very Good) Required test</t>
+  </si>
+  <si>
+    <t>Rate your overall experience (1 - Very Poor, 5 - Very Good) options test</t>
+  </si>
+  <si>
+    <t>Would you recommend us to your friends? Style</t>
+  </si>
+  <si>
+    <t>Would you recommend us to your friends? User selects no</t>
+  </si>
+  <si>
+    <t>First Name style</t>
+  </si>
+  <si>
+    <t>First name requirement</t>
+  </si>
+  <si>
+    <t>will not submit</t>
+  </si>
+  <si>
+    <t>Last name style</t>
+  </si>
+  <si>
+    <t>Last name requirement</t>
+  </si>
+  <si>
+    <t>Email style</t>
+  </si>
+  <si>
+    <t>characters can no longer be added</t>
+  </si>
+  <si>
+    <t>Email max 32 characters</t>
+  </si>
+  <si>
+    <t>Email requirement</t>
+  </si>
+  <si>
+    <t>Phone number style</t>
+  </si>
+  <si>
+    <t>Phone Number: 14 px // Arial. Left justified. Ghost text: “Phone Number”.</t>
+  </si>
+  <si>
+    <t>characters cannot be added</t>
+  </si>
+  <si>
+    <t>Please fill out this field popup style</t>
+  </si>
+  <si>
+    <t>Pop up shows up</t>
+  </si>
+  <si>
+    <t>TC37</t>
+  </si>
+  <si>
+    <t>TC38</t>
+  </si>
+  <si>
+    <t>TC39</t>
+  </si>
+  <si>
+    <t>TC40</t>
+  </si>
+  <si>
+    <t>TC41</t>
+  </si>
+  <si>
+    <t>TC42</t>
+  </si>
+  <si>
+    <t>TC43</t>
+  </si>
+  <si>
+    <t>TC44</t>
+  </si>
+  <si>
+    <t>TC45</t>
+  </si>
+  <si>
+    <t>TC46</t>
+  </si>
+  <si>
+    <t>TC47</t>
+  </si>
+  <si>
+    <t>TC48</t>
+  </si>
+  <si>
+    <t>Submit button style</t>
+  </si>
+  <si>
+    <t>24pt / Arial Right Justified</t>
+  </si>
+  <si>
+    <t>Submit button function</t>
+  </si>
+  <si>
+    <t>Overall style guide</t>
+  </si>
+  <si>
+    <t>1. All text boxes have drop shadows
+2. Left justified fields should line up on left.
+3. Right justified fields should line up on right.
+4. Similar Options should line up together</t>
+  </si>
+  <si>
+    <t>Mobile Style</t>
+  </si>
+  <si>
+    <t>Analytics Tracking:
+Page Visit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analytics Tracking:
+Mailing List </t>
+  </si>
+  <si>
+    <t>Analytics Tracking:
+Form Submit</t>
+  </si>
+  <si>
+    <t>Google Analytics Debugger returns a message about the Mailing List link being clicked being tracked on the dev console</t>
+  </si>
+  <si>
+    <t>Google Analytics Debugger returns a message about the page visit being tracked on the dev console</t>
+  </si>
+  <si>
+    <t>1. Visit the site in each browser
+2. Fill out the form with valid inputs
+3. Submit the form
+4. Expect output 1
+5. Click the mailing link
+6. Expect output 2
+7. Fill out the mailing list form and submit
+8. Expect output 3</t>
+  </si>
+  <si>
+    <t>1. Visit Site</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Hover over mailing list link</t>
+  </si>
+  <si>
+    <t>Mailing list link style and hover</t>
+  </si>
+  <si>
+    <t>Mailing list link click</t>
+  </si>
+  <si>
+    <t>“Sign Up for Our Newsletter” pop-up appears.</t>
+  </si>
+  <si>
+    <t>Email max field length in signup newsletter popup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Visit Site
+2. Click on mailing list link </t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Click on mailing list link
+3. Enter a 255 character string and then try to type in one more character</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validates all required values are present, submits
+the page if no errors are present. Closes the pop up.</t>
+  </si>
+  <si>
+    <t>Close mailing list popup</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Click on mailing list link
+3. Fill out email field with a valid email
+4. Do not tick off the 18 or older field</t>
+  </si>
+  <si>
+    <t>1. Visit site
+2. Click on mailing list link
+3. Click on X to close popup</t>
+  </si>
+  <si>
+    <t>Popup is closed</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Fill out form but leave First name blank
+3. Submit form</t>
+  </si>
+  <si>
+    <t>Popup should show up in the name field and have this style: 20pt / Arial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Visit Site using mobile devices listed below:
+-iPhones 5-7
+-Galaxy S5-S7
+</t>
+  </si>
+  <si>
+    <t>1. Open chrome developer tools and navigate to the console
+2. Visit page</t>
+  </si>
+  <si>
+    <t>1. Open chrome developer tools and navigate to the console
+2. Visit page
+3. Click on the mailing list link</t>
+  </si>
+  <si>
+    <t>Analytics Tracking:
+Mailing List Submission</t>
+  </si>
+  <si>
+    <t>1. Open chrome developer tools and navigate to the console
+2. Visit page
+3. Click on the mailing list link
+4. Fill out and submit form with valid inputs</t>
+  </si>
+  <si>
+    <t>1. Open chrome developer tools and navigate to the console
+2. Visit page
+3. Fill out and submit feedback for with valid inputs</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Fill out form with valid inputs
+3. Click on submit button</t>
+  </si>
+  <si>
+    <t>Please fill out this field pop up functionality with one missing field</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Attempt to type non number characters in the phone number field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Visit Site
+2. Enter 32 number characters in the phone number field
+3. Try to enter in a 33rd character in the phone number field </t>
+  </si>
+  <si>
+    <t>1. Visit site
+2. Fill out form but leave the email field blank
+3. Submit form</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Fill out email field with 32 characters
+3. Try to enter in a 33rd character</t>
+  </si>
+  <si>
+    <t>1. Visit site 
+2. Fill out form but leave last name field blank
+3. Submit form</t>
+  </si>
+  <si>
+    <t>1. Visit site 
+2. Fill out form but leave first name field blank
+3. Submit form</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Try to check off more then one option in the how did you hear about us field</t>
+  </si>
+  <si>
+    <t>Should not be able to add another character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Visit Site
+2. Select other in how you heard about us field
+3. Enter a 32 character string
+4. Try to add a 33rd character </t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Select other in how you heard about us
+3. Enter a valid string
+4. Fill out the rest of the form with valid inputs
+5. Submit form</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The field style should be 28 px / Arial. Left justified. Options (14px /
+Arial): 1 / 2 / 3 / 4 / 5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The field style should be 18 px / Arial. Left justified Options (14 px / Arial): Yes / No.</t>
+  </si>
+  <si>
+    <t>Mailing list style: 21 px / Arial. Hover over turns the text yellow.</t>
+  </si>
+  <si>
+    <t>Company motto style: 21 px / Arial / italic. Horizontally centered inside the header, below the company name.</t>
+  </si>
+  <si>
+    <t>Company logo style: Vertically centered within header. 15px from left edge.</t>
+  </si>
+  <si>
+    <t>Popup style:
+1. Sign Up for Out Newsletter text: 18 px / Arial. Horizontally centered within the pop-up
+2. Email Address field should contain ghost text: “Email Address”. Horizontally centered within the pop-up
+3. I certify that I am 18 years of age or older text: 18px/ Arial. Horizontally centered within the pop-up.
 4. Sign Up: Horizontally centered within the pop-up.
 5. Close X is right justified</t>
   </si>
   <si>
-    <t>“Sign Up for Our Newsletter” pop-up.</t>
-  </si>
-  <si>
-    <t>Email max field length</t>
-  </si>
-  <si>
-    <t>no more characters can be added</t>
-  </si>
-  <si>
-    <t>Email Validation: format</t>
-  </si>
-  <si>
-    <t>emails of incorrect format should not be able to submit</t>
-  </si>
-  <si>
-    <t>• Email must be in the format of “local@domain”
-• The localpart must be 64 characters or less.
-• The domain must have a “.” to differentiate the domain from the TLD, i.e. “domain.ld”
-• Can only contain a-z, A-Z, 0-9, or any of !#$%&amp;'*+-/=?^_`{|}~.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> I certify that I am 18 years of age or older has to be ticked</t>
-  </si>
-  <si>
-    <t>should not be able to submit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Validates all required values are present, submits
-the page if no errors are present. Closes the pop up if successful.</t>
-  </si>
-  <si>
-    <t>Signup with valid credentials</t>
-  </si>
-  <si>
-    <t>How did you hear about ACME VC&amp;A Co.?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 18 px / Arial. Left justified. Options (14px / arial): Social
+    <t>No more characters can be added</t>
+  </si>
+  <si>
+    <t>Emails of incorrect format should not be able to submit</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Fill out first name field with 32 character string
+3. Attempt to add a 33rd character</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Style: 14 px / Arial. Left justified. Ghost text: “First Name”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Style: 14 px / Arial. Left justified. Ghost text: “Last Name”. </t>
+  </si>
+  <si>
+    <t>Style: 14 px / Arial. Left justified. Ghost text: “Email”.</t>
+  </si>
+  <si>
+    <t>Last name max 32 chars</t>
+  </si>
+  <si>
+    <t>First name max length 32 chars</t>
+  </si>
+  <si>
+    <t>Would you recommend us to your friends? User selects no max char length 100</t>
+  </si>
+  <si>
+    <t>Would you recommend us to your friends? User selects no but leaves blank</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Form is submitted successfully</t>
+  </si>
+  <si>
+    <t>1. Form is able to be successfully submitted 
+2. Mailing list link click returns the popup for signing up 
+3. Mailing list signup can be successfully done</t>
+  </si>
+  <si>
+    <t>Company motto</t>
+  </si>
+  <si>
+    <t>Company name style: 30 px / Arial. Horizontally centered inside the header, above the company motto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Visit Site
+2. Click on mailing list link
+3. Enter string that does not follow the conventional email format "local@domain.id" either by not having an "@" or by not having a "." to  differentiate the domain from the TLD.
+4. Expect output
+5. Type in an email where the local part of local@domain is longer the 64 chars
+6. Expect output
+7. Enter an email that contains a character not listed here  :a-z, A-Z, 0-9, or any of !#$%&amp;'*+-/=?^_`{|}~.
+8. Expect output
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18 px / Arial. Left justified. Options (14px / Arial): Social
 media / Advertising / Search Engine / Friend / Other. Default = Social Media.</t>
   </si>
   <si>
-    <t>How did you hear about ACME VC&amp;A Co.? Buttons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only one should be able to be selected. </t>
-  </si>
-  <si>
-    <t>How did you hear about ACME VC&amp;A Co.? Other Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Other: Ghost text: “Other”. Max length: 32 chars. Text field is required if “Other” radio button is
-selected."  </t>
-  </si>
-  <si>
-    <t>Should not be able to submit</t>
-  </si>
-  <si>
-    <t>How did you hear about ACME VC&amp;A Co.? Other Field passing</t>
-  </si>
-  <si>
-    <t>Should be able to submit</t>
-  </si>
-  <si>
-    <t>Rate your overall experience (1 - Very Poor, 5 - Very Good): Styling</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 28 px / Arial. Left justified. Options (14px /
-Arial): 1 / 2 / 3 / 4 / 5.</t>
-  </si>
-  <si>
-    <t>Only one option can be selected</t>
-  </si>
-  <si>
-    <t>Rate your overall experience (1 - Very Poor, 5 - Very Good) Required test</t>
-  </si>
-  <si>
-    <t>Rate your overall experience (1 - Very Poor, 5 - Very Good) options test</t>
-  </si>
-  <si>
-    <t>Would you recommend us to your friends? Style</t>
-  </si>
-  <si>
-    <t>18 px / Arial. Left justified Options (14 px / Arial): Yes / No.</t>
-  </si>
-  <si>
-    <t>Would you recommend us to your friends? User selects no</t>
-  </si>
-  <si>
-    <t>If user selects “No” in under “Would you recommend us to your
-friends?” show this question and field. Max field length: 100. Required if ‘No’ is selected in “Would you
-recommend us to your friends?”.</t>
-  </si>
-  <si>
-    <t>First Name style</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 14 px / Arial. Left justified. Ghost text: “Last Name”. Max length: 32 chars.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 14 px / Arial. Left justified. Ghost text: “First Name”. Max length: 32 chars.</t>
-  </si>
-  <si>
-    <t>First name requirement</t>
-  </si>
-  <si>
-    <t>will not submit</t>
-  </si>
-  <si>
-    <t>Last name style</t>
-  </si>
-  <si>
-    <t>Last name requirement</t>
-  </si>
-  <si>
-    <t>Email style</t>
-  </si>
-  <si>
-    <t>14 px / Arial. Left justified. Ghost text: “Email”.</t>
-  </si>
-  <si>
-    <t>characters can no longer be added</t>
-  </si>
-  <si>
-    <t>Email max 32 characters</t>
-  </si>
-  <si>
-    <t>Email requirement</t>
-  </si>
-  <si>
-    <t>Phone number style</t>
-  </si>
-  <si>
-    <t>Phone Number: 14 px // Arial. Left justified. Ghost text: “Phone Number”.</t>
-  </si>
-  <si>
-    <t>Phone numer max 32 chars</t>
+    <t>1. Visit Site
+2. Attempt to click more the one option in the rate your overall experience field</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Leave the rate your overall experience field blank
+3. Fill out the rest of feedback form with valid inputs
+4. Submit form</t>
+  </si>
+  <si>
+    <t>1. Visit Site 
+2. Click no on the recommend to friends field
+3. Fill in with 100 character string
+4. Attempt to add a 101st character</t>
+  </si>
+  <si>
+    <t>1. Visit Site 
+2. Click no on the recommend to friends field
+3. Leave text field blank
+4. Fill out the rest of the form with valid input
+5. Submit form</t>
+  </si>
+  <si>
+    <t>1. Visit Site 
+2. Click no on the recommend to friends field
+3. Fill  in text field with less then 100 chars
+4. Fill out the rest of the form with valid inputs
+5. Submit form</t>
+  </si>
+  <si>
+    <t>Phone number max 32 chars</t>
+  </si>
+  <si>
+    <t>Phone number only numbers can be added</t>
+  </si>
+  <si>
+    <t>1. Submits all the information
+2. Successful form submission popup appears</t>
+  </si>
+  <si>
+    <t>Google Analytics Debugger returns a message about the form being successfully submitted on the dev console</t>
+  </si>
+  <si>
+    <t>fails on mozzilla all the user rating input buttons are required</t>
+  </si>
+  <si>
+    <t>logo is not vertically centered in the header</t>
+  </si>
+  <si>
+    <t>1. Visit the site
+2. Inspect the element using the dev tools</t>
+  </si>
+  <si>
+    <t>1. Visit the site
+2. Resize browser to check if the logo scales correctly
+3. Inspect the element using the dev tools</t>
+  </si>
+  <si>
+    <t>hover over only part of the text turns yellow on hover</t>
+  </si>
+  <si>
+    <t>Email address ghost text is incorrect
+I certify that I am 18 years or older font size is 14px instead of 18px
+Sign up button is not horizontally centered</t>
+  </si>
+  <si>
+    <t>valid email fails after having input a wrong email</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Click on mailing list link
+3. Fill out email field with a valid email
+4. Check off the 18 or older option 
+5. Submit form
+6. Expect result
+7. Click on mailing list link
+8. Fill out with invalid email
+9. Check off 18 or older option
+10. Expect result</t>
+  </si>
+  <si>
+    <t>Form was closed</t>
+  </si>
+  <si>
+    <t>1. Visit Site
+2. Inspect element with dev tools</t>
+  </si>
+  <si>
+    <t>font size is 18px but might be a typo in the requirements sheet</t>
+  </si>
+  <si>
+    <t>multiple options can be selected</t>
+  </si>
+  <si>
+    <t>Why not option is not formatted correctly</t>
+  </si>
+  <si>
+    <t>form submits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address is incorrectly spelt and the ghost text has a conflict in the PRD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows ( ) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not the right font size </t>
+  </si>
+  <si>
+    <t>Contact information Style</t>
+  </si>
+  <si>
+    <t>Arial font</t>
+  </si>
+  <si>
+    <t>The font is incorrect. It is not specified in PRD but is not consitent with the style of page.</t>
+  </si>
+  <si>
+    <t>Field headers</t>
+  </si>
+  <si>
+    <t>1.Visist Site
+2. Inspect the titles for each field with the dev tools</t>
+  </si>
+  <si>
+    <t>Text should have Arail font.</t>
+  </si>
+  <si>
+    <t>Text is bold</t>
+  </si>
+  <si>
+    <t>Font size is incorrect</t>
+  </si>
+  <si>
+    <t>Should have the same results as:
+TC3
+TC4
+TC5
+TC36
+TC43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logo is not aligned
+Header does not go all the way to edge of screen
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Mailing list popup email text box does not have a drop shadow
+2. Last name and phone number fields are not aligned
+</t>
+  </si>
+  <si>
+    <t>Data did not save</t>
+  </si>
+  <si>
+    <t>No message regarding if the form was saved or not</t>
   </si>
 </sst>
 </file>
@@ -584,7 +871,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -715,23 +1002,10 @@
       <charset val="128"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <charset val="128"/>
     </font>
     <font>
       <u/>
@@ -747,8 +1021,14 @@
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -769,18 +1049,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="41"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="56"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -788,6 +1056,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="61"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1240,39 +1514,149 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1477,7 +1861,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1493,10 +1877,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1512,22 +1892,12 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1546,15 +1916,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1564,37 +1925,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1618,17 +1976,31 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="30">
+  <cellStyles count="140">
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
@@ -1642,6 +2014,61 @@
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -1655,6 +2082,61 @@
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Functional Test Case v1.0" xfId="1"/>
     <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="2"/>
@@ -4254,7 +4736,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4276,7 +4758,7 @@
     <row r="2" spans="1:7" ht="23">
       <c r="A2" s="26"/>
       <c r="B2" s="27" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -4287,7 +4769,7 @@
     <row r="3" spans="1:7">
       <c r="A3" s="26"/>
       <c r="B3" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="60">
         <v>1</v>
@@ -4300,7 +4782,7 @@
     <row r="4" spans="1:7">
       <c r="A4" s="26"/>
       <c r="B4" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="11">
         <v>42850</v>
@@ -4322,13 +4804,13 @@
     <row r="6" spans="1:7" ht="14.25" customHeight="1">
       <c r="A6" s="26"/>
       <c r="B6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="111" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="111"/>
-      <c r="E6" s="112"/>
+        <v>37</v>
+      </c>
+      <c r="C6" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="105"/>
+      <c r="E6" s="106"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
@@ -4352,27 +4834,27 @@
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="36" customFormat="1" ht="26">
       <c r="B10" s="49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="50" t="s">
-        <v>15</v>
-      </c>
       <c r="F10" s="50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="36" customFormat="1">
@@ -4380,26 +4862,26 @@
         <v>42850</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="74" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="36" customFormat="1">
-      <c r="B12" s="107"/>
+      <c r="B12" s="101"/>
       <c r="C12" s="39"/>
       <c r="D12" s="40"/>
       <c r="E12" s="41"/>
       <c r="F12" s="74"/>
-      <c r="G12" s="105"/>
+      <c r="G12" s="100"/>
     </row>
     <row r="13" spans="1:7" s="37" customFormat="1" ht="13">
       <c r="B13" s="38"/>
@@ -4407,7 +4889,7 @@
       <c r="D13" s="40"/>
       <c r="E13" s="41"/>
       <c r="F13" s="74"/>
-      <c r="G13" s="105"/>
+      <c r="G13" s="100"/>
     </row>
     <row r="14" spans="1:7" s="37" customFormat="1" ht="13">
       <c r="B14" s="44"/>
@@ -4504,10 +4986,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N86"/>
+  <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" outlineLevelRow="1" x14ac:dyDescent="0"/>
@@ -4518,579 +5000,651 @@
     <col min="6" max="6" width="23.6640625" customWidth="1"/>
     <col min="7" max="7" width="18.5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="96"/>
-    <col min="10" max="10" width="18" style="94" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="94"/>
+    <col min="10" max="10" width="18" style="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
+        <v>77</v>
+      </c>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="109"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="103"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="109"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="103"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="111" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="112"/>
+        <v>38</v>
+      </c>
+      <c r="B3" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="105"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="65"/>
       <c r="F3" s="65"/>
       <c r="G3" s="65"/>
-      <c r="H3" s="133"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="14">
       <c r="A4" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="134" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="135"/>
-      <c r="D4" s="136"/>
+        <v>39</v>
+      </c>
+      <c r="B4" s="124" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="125"/>
+      <c r="D4" s="126"/>
       <c r="E4" s="65"/>
       <c r="F4" s="65"/>
       <c r="G4" s="65"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="87">
+        <f>COUNTIF(I11:I50,"Pass")</f>
+        <v>23</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="87">
-        <f>COUNTIF(I11:I45,"Pass")</f>
-        <v>25</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="D5" s="13">
-        <f>COUNTIF(I9:I767,"Pending")</f>
+        <f>COUNTIF(I9:I762,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
       <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="88">
-        <f>COUNTIF(I11:I45,"Fail")</f>
-        <v>1</v>
+        <f>COUNTIF(I11:I50,"Fail")</f>
+        <v>17</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="63">
-        <f>COUNTA(A11:A48) -15</f>
-        <v>23</v>
+        <f>COUNTA(A11:A57)</f>
+        <v>47</v>
       </c>
       <c r="E6" s="66"/>
       <c r="F6" s="66"/>
       <c r="G6" s="66"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="123"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="132"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
+      <c r="A7" s="122"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="77" customFormat="1" ht="12" customHeight="1">
-      <c r="A8" s="120" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="122" t="s">
+      <c r="A8" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="112" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="110" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="114" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="115"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="127" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="120" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="124" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="137" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="121" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="121" t="s">
-        <v>97</v>
+      <c r="J8" s="111" t="s">
+        <v>182</v>
       </c>
       <c r="K8" s="76"/>
     </row>
     <row r="9" spans="1:11" s="68" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="121"/>
-      <c r="B9" s="123"/>
-      <c r="C9" s="121"/>
-      <c r="D9" s="127"/>
-      <c r="E9" s="128"/>
-      <c r="F9" s="128"/>
-      <c r="G9" s="129"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="121"/>
-      <c r="J9" s="121"/>
+      <c r="A9" s="111"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="111"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="119"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
       <c r="K9" s="67"/>
     </row>
     <row r="10" spans="1:11" s="78" customFormat="1" ht="18">
-      <c r="A10" s="138"/>
-      <c r="B10" s="138"/>
-      <c r="C10" s="138"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="138"/>
-      <c r="I10" s="138"/>
-      <c r="J10" s="139"/>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="26" outlineLevel="1">
+      <c r="A10" s="128" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="128"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="129"/>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="117" customHeight="1" outlineLevel="1">
       <c r="A11" s="82" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C11" s="81" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="116" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
+        <v>132</v>
+      </c>
+      <c r="D11" s="107" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="108"/>
+      <c r="F11" s="108"/>
       <c r="G11" s="80"/>
-      <c r="H11" s="103"/>
+      <c r="H11" s="131">
+        <v>42850</v>
+      </c>
       <c r="I11" s="81" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="J11" s="79" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A12" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="97" t="s">
-        <v>98</v>
-      </c>
-      <c r="C12" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="119" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
+      <c r="B12" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="107" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="108"/>
+      <c r="F12" s="108"/>
       <c r="G12" s="80"/>
-      <c r="H12" s="92"/>
+      <c r="H12" s="131">
+        <v>42850</v>
+      </c>
       <c r="I12" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="79"/>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+        <v>9</v>
+      </c>
+      <c r="J12" s="79" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
       <c r="A13" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="97" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="116" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
+      <c r="B13" s="95" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" s="96" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="107" t="s">
+        <v>169</v>
+      </c>
+      <c r="E13" s="108"/>
+      <c r="F13" s="108"/>
       <c r="G13" s="80"/>
-      <c r="H13" s="103"/>
+      <c r="H13" s="131">
+        <v>42850</v>
+      </c>
       <c r="I13" s="81" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13" s="79"/>
     </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="36" customHeight="1" outlineLevel="1">
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="28" customHeight="1" outlineLevel="1">
       <c r="A14" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="97" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="116" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="117"/>
-      <c r="F14" s="117"/>
+      <c r="B14" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="96" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" s="107" t="s">
+        <v>186</v>
+      </c>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
       <c r="G14" s="80"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="81"/>
+      <c r="H14" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I14" s="81" t="s">
+        <v>40</v>
+      </c>
       <c r="J14" s="79"/>
     </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="28" customHeight="1" outlineLevel="1">
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A15" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="97" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117"/>
+      <c r="B15" s="95" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="96" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="107" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="108"/>
+      <c r="F15" s="108"/>
       <c r="G15" s="80"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="79"/>
+      <c r="H15" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I15" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="79" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A16" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="97" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="96" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="107" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="108"/>
+      <c r="F16" s="108"/>
       <c r="G16" s="80"/>
-      <c r="H16" s="92"/>
+      <c r="H16" s="131">
+        <v>42850</v>
+      </c>
       <c r="I16" s="81" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" s="79"/>
     </row>
-    <row r="17" spans="1:14" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+    <row r="17" spans="1:14" s="4" customFormat="1" ht="138" customHeight="1" outlineLevel="1">
       <c r="A17" s="82" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="95" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="96" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="107" t="s">
+        <v>171</v>
+      </c>
+      <c r="E17" s="108"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I17" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="97" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="116" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="103"/>
-      <c r="I17" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="79"/>
-    </row>
-    <row r="18" spans="1:14" s="4" customFormat="1" ht="138" customHeight="1" outlineLevel="1">
+      <c r="J17" s="79" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="4" customFormat="1" ht="60" customHeight="1" outlineLevel="1">
       <c r="A18" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="97" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="116" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="B18" s="95" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="96" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="107" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
       <c r="G18" s="80"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="81"/>
+      <c r="H18" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I18" s="81" t="s">
+        <v>40</v>
+      </c>
       <c r="J18" s="79"/>
     </row>
-    <row r="19" spans="1:14" s="4" customFormat="1" ht="35" customHeight="1" outlineLevel="1">
+    <row r="19" spans="1:14" s="85" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
       <c r="A19" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="97" t="s">
-        <v>112</v>
-      </c>
-      <c r="C19" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="116" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="92"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="79"/>
-    </row>
-    <row r="20" spans="1:14" s="85" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
+      <c r="B19" s="90" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="84" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" s="107" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="H19" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I19" s="99" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="99"/>
+    </row>
+    <row r="20" spans="1:14" s="85" customFormat="1" ht="69" customHeight="1" outlineLevel="1">
       <c r="A20" s="82" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="90" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C20" s="84" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="116" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" s="117"/>
-      <c r="F20" s="117"/>
-      <c r="I20" s="104" t="s">
-        <v>41</v>
-      </c>
-      <c r="J20" s="86"/>
-    </row>
-    <row r="21" spans="1:14" s="85" customFormat="1" ht="69" customHeight="1" outlineLevel="1">
+        <v>143</v>
+      </c>
+      <c r="D20" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="108"/>
+      <c r="F20" s="108"/>
+      <c r="H20" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I20" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="85" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="85" customFormat="1" ht="82" customHeight="1" outlineLevel="1">
       <c r="A21" s="82" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="90" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="C21" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
-      <c r="H21" s="102"/>
-      <c r="I21" s="104" t="s">
-        <v>41</v>
-      </c>
-      <c r="J21" s="86"/>
+        <v>205</v>
+      </c>
+      <c r="D21" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
+      <c r="H21" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I21" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="99" t="s">
+        <v>204</v>
+      </c>
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="97"/>
+      <c r="N21" s="97"/>
     </row>
     <row r="22" spans="1:14" s="85" customFormat="1" ht="56" customHeight="1" outlineLevel="1">
       <c r="A22" s="82" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="90" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="C22" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="116" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="117"/>
-      <c r="F22" s="117"/>
-      <c r="H22" s="102"/>
-      <c r="I22" s="100"/>
-      <c r="J22" s="101"/>
-      <c r="K22" s="99"/>
-      <c r="L22" s="99"/>
-      <c r="M22" s="99"/>
-      <c r="N22" s="99"/>
+        <v>144</v>
+      </c>
+      <c r="D22" s="107" t="s">
+        <v>145</v>
+      </c>
+      <c r="E22" s="108"/>
+      <c r="F22" s="108"/>
+      <c r="H22" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I22" s="98" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="134"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="97"/>
     </row>
     <row r="23" spans="1:14" s="85" customFormat="1" ht="65" customHeight="1" outlineLevel="1">
       <c r="A23" s="82" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="90" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
       <c r="C23" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="116" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" s="117"/>
-      <c r="F23" s="117"/>
-      <c r="H23" s="93"/>
-      <c r="I23" s="95"/>
-      <c r="J23" s="86"/>
+        <v>207</v>
+      </c>
+      <c r="D23" s="107" t="s">
+        <v>188</v>
+      </c>
+      <c r="E23" s="108"/>
+      <c r="F23" s="108"/>
+      <c r="H23" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I23" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="79"/>
     </row>
     <row r="24" spans="1:14" s="85" customFormat="1" ht="70.5" customHeight="1" outlineLevel="1">
       <c r="A24" s="82" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="90" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="C24" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="116" t="s">
-        <v>124</v>
-      </c>
-      <c r="E24" s="117"/>
-      <c r="F24" s="117"/>
-      <c r="H24" s="93"/>
-      <c r="I24" s="95" t="s">
-        <v>41</v>
+        <v>162</v>
+      </c>
+      <c r="D24" s="107" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="108"/>
+      <c r="F24" s="108"/>
+      <c r="H24" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I24" s="93" t="s">
+        <v>40</v>
       </c>
       <c r="J24" s="86"/>
     </row>
     <row r="25" spans="1:14" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A25" s="82" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="B25" s="90" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="C25" s="84" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="116" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" s="117"/>
-      <c r="F25" s="117"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="95" t="s">
-        <v>41</v>
+        <v>164</v>
+      </c>
+      <c r="D25" s="107" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="108"/>
+      <c r="F25" s="108"/>
+      <c r="H25" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I25" s="93" t="s">
+        <v>40</v>
       </c>
       <c r="J25" s="86"/>
     </row>
     <row r="26" spans="1:14" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A26" s="82" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26" s="90" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="C26" s="84" t="s">
-        <v>126</v>
-      </c>
-      <c r="D26" s="116" t="s">
-        <v>129</v>
-      </c>
-      <c r="E26" s="117"/>
-      <c r="F26" s="117"/>
-      <c r="H26" s="93"/>
-      <c r="I26" s="95" t="s">
-        <v>41</v>
+        <v>165</v>
+      </c>
+      <c r="D26" s="107" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
+      <c r="H26" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I26" s="93" t="s">
+        <v>40</v>
       </c>
       <c r="J26" s="86"/>
     </row>
     <row r="27" spans="1:14" s="85" customFormat="1" ht="59.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="82" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" s="90" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="C27" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="116" t="s">
-        <v>131</v>
-      </c>
-      <c r="E27" s="117"/>
-      <c r="F27" s="117"/>
-      <c r="H27" s="93"/>
-      <c r="I27" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J27" s="86"/>
+        <v>133</v>
+      </c>
+      <c r="D27" s="107" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="108"/>
+      <c r="F27" s="108"/>
+      <c r="H27" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I27" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="130" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="28" spans="1:14" s="85" customFormat="1" ht="56.25" customHeight="1" outlineLevel="1">
       <c r="A28" s="82" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B28" s="90" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
       <c r="C28" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="116" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="117"/>
-      <c r="F28" s="117"/>
-      <c r="H28" s="93"/>
-      <c r="I28" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J28" s="86"/>
+        <v>189</v>
+      </c>
+      <c r="D28" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="108"/>
+      <c r="F28" s="108"/>
+      <c r="H28" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I28" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="99" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="29" spans="1:14" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A29" s="82" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="90" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
       <c r="C29" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="116" t="s">
-        <v>127</v>
-      </c>
-      <c r="E29" s="117"/>
-      <c r="F29" s="117"/>
-      <c r="H29" s="93"/>
-      <c r="I29" s="95" t="s">
-        <v>41</v>
+        <v>190</v>
+      </c>
+      <c r="D29" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="108"/>
+      <c r="F29" s="108"/>
+      <c r="H29" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I29" s="93" t="s">
+        <v>40</v>
       </c>
       <c r="J29" s="86"/>
     </row>
@@ -5099,429 +5653,819 @@
         <v>53</v>
       </c>
       <c r="B30" s="90" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="C30" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="116" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" s="117"/>
-      <c r="F30" s="117"/>
-      <c r="H30" s="93"/>
-      <c r="I30" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J30" s="86"/>
-    </row>
-    <row r="31" spans="1:14" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+        <v>207</v>
+      </c>
+      <c r="D30" s="107" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" s="108"/>
+      <c r="F30" s="108"/>
+      <c r="H30" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I30" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="130" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="85" customFormat="1" ht="62.25" customHeight="1" outlineLevel="1">
       <c r="A31" s="82" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="90" t="s">
-        <v>137</v>
+        <v>180</v>
       </c>
       <c r="C31" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="116" t="s">
-        <v>138</v>
-      </c>
-      <c r="E31" s="117"/>
-      <c r="F31" s="117"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J31" s="86"/>
-    </row>
-    <row r="32" spans="1:14" s="85" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
+        <v>191</v>
+      </c>
+      <c r="D31" s="107" t="s">
+        <v>163</v>
+      </c>
+      <c r="E31" s="108"/>
+      <c r="F31" s="108"/>
+      <c r="H31" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I31" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J31" s="130"/>
+    </row>
+    <row r="32" spans="1:14" s="85" customFormat="1" ht="74" customHeight="1" outlineLevel="1">
       <c r="A32" s="82" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="90" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="C32" s="84" t="s">
+        <v>192</v>
+      </c>
+      <c r="D32" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="108"/>
+      <c r="F32" s="108"/>
+      <c r="H32" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I32" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="130"/>
+    </row>
+    <row r="33" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A33" s="82" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="84" t="s">
+        <v>193</v>
+      </c>
+      <c r="D33" s="107" t="s">
+        <v>183</v>
+      </c>
+      <c r="E33" s="108"/>
+      <c r="F33" s="108"/>
+      <c r="H33" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I33" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J33" s="86"/>
+    </row>
+    <row r="34" spans="1:10" s="85" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
+      <c r="A34" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="116" t="s">
-        <v>141</v>
-      </c>
-      <c r="E32" s="117"/>
-      <c r="F32" s="117"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="106" t="s">
-        <v>10</v>
-      </c>
-      <c r="J32" s="86" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="85" customFormat="1" ht="96" customHeight="1" outlineLevel="1">
-      <c r="A33" s="82" t="s">
+      <c r="C34" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="107" t="s">
+        <v>175</v>
+      </c>
+      <c r="E34" s="108"/>
+      <c r="F34" s="108"/>
+      <c r="H34" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I34" s="132" t="s">
+        <v>40</v>
+      </c>
+      <c r="J34" s="130"/>
+    </row>
+    <row r="35" spans="1:10" s="85" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
+      <c r="A35" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="90" t="s">
+        <v>179</v>
+      </c>
+      <c r="C35" s="84" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="107" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" s="108"/>
+      <c r="F35" s="108"/>
+      <c r="H35" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I35" s="132" t="s">
+        <v>40</v>
+      </c>
+      <c r="J35" s="130"/>
+    </row>
+    <row r="36" spans="1:10" s="85" customFormat="1" ht="96" customHeight="1" outlineLevel="1">
+      <c r="A36" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="90" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="84" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="108"/>
+      <c r="F36" s="108"/>
+      <c r="H36" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I36" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J36" s="86"/>
+    </row>
+    <row r="37" spans="1:10" s="85" customFormat="1" ht="96" customHeight="1" outlineLevel="1">
+      <c r="A37" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="90" t="s">
-        <v>142</v>
-      </c>
-      <c r="C33" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="116" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="117"/>
-      <c r="F33" s="117"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J33" s="86" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="85" customFormat="1" ht="96" customHeight="1" outlineLevel="1">
-      <c r="A34" s="82" t="s">
+      <c r="B37" s="90" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="84" t="s">
+        <v>207</v>
+      </c>
+      <c r="D37" s="107" t="s">
+        <v>176</v>
+      </c>
+      <c r="E37" s="108"/>
+      <c r="F37" s="108"/>
+      <c r="H37" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I37" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J37" s="130"/>
+    </row>
+    <row r="38" spans="1:10" s="85" customFormat="1" ht="96" customHeight="1" outlineLevel="1">
+      <c r="A38" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="90" t="s">
-        <v>144</v>
-      </c>
-      <c r="C34" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="D34" s="116" t="s">
-        <v>140</v>
-      </c>
-      <c r="E34" s="117"/>
-      <c r="F34" s="117"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J34" s="86" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="85" customFormat="1" ht="27.75" customHeight="1" outlineLevel="1">
-      <c r="A35" s="82" t="s">
+      <c r="B38" s="90" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="84" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="107" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="108"/>
+      <c r="F38" s="108"/>
+      <c r="H38" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I38" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J38" s="130"/>
+    </row>
+    <row r="39" spans="1:10" s="85" customFormat="1" ht="50" customHeight="1" outlineLevel="1">
+      <c r="A39" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="90" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="84"/>
-      <c r="D35" s="116" t="s">
-        <v>143</v>
-      </c>
-      <c r="E35" s="117"/>
-      <c r="F35" s="117"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J35" s="86"/>
-    </row>
-    <row r="36" spans="1:10" s="85" customFormat="1" ht="81" customHeight="1" outlineLevel="1">
-      <c r="A36" s="82" t="s">
+      <c r="B39" s="90" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="84" t="s">
+        <v>160</v>
+      </c>
+      <c r="D39" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="108"/>
+      <c r="F39" s="108"/>
+      <c r="H39" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I39" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39" s="99" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="85" customFormat="1" ht="81" customHeight="1" outlineLevel="1">
+      <c r="A40" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="90" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" s="84"/>
-      <c r="D36" s="118" t="s">
-        <v>147</v>
-      </c>
-      <c r="E36" s="117"/>
-      <c r="F36" s="117"/>
-      <c r="H36" s="93"/>
-      <c r="I36" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J36" s="86"/>
-    </row>
-    <row r="37" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
-      <c r="A37" s="82" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="90" t="s">
-        <v>149</v>
-      </c>
-      <c r="C37" s="84"/>
-      <c r="D37" s="116" t="s">
-        <v>148</v>
-      </c>
-      <c r="E37" s="117"/>
-      <c r="F37" s="117"/>
-      <c r="H37" s="93"/>
-      <c r="I37" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" s="86"/>
-    </row>
-    <row r="38" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
-      <c r="A38" s="82" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="90" t="s">
-        <v>150</v>
-      </c>
-      <c r="C38" s="84"/>
-      <c r="D38" s="116" t="s">
-        <v>143</v>
-      </c>
-      <c r="E38" s="117"/>
-      <c r="F38" s="117"/>
-      <c r="H38" s="93"/>
-      <c r="I38" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J38" s="86"/>
-    </row>
-    <row r="39" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
-      <c r="A39" s="82" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="90" t="s">
-        <v>151</v>
-      </c>
-      <c r="C39" s="84"/>
-      <c r="D39" s="116" t="s">
-        <v>152</v>
-      </c>
-      <c r="E39" s="117"/>
-      <c r="F39" s="117"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="86"/>
-    </row>
-    <row r="40" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
-      <c r="A40" s="82" t="s">
-        <v>67</v>
-      </c>
       <c r="B40" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" s="84"/>
-      <c r="D40" s="116" t="s">
-        <v>148</v>
-      </c>
-      <c r="E40" s="117"/>
-      <c r="F40" s="117"/>
-      <c r="H40" s="93"/>
-      <c r="I40" s="95"/>
-      <c r="J40" s="86"/>
+        <v>100</v>
+      </c>
+      <c r="C40" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="109" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" s="133"/>
+      <c r="F40" s="133"/>
+      <c r="H40" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I40" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J40" s="130" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="41" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A41" s="82" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B41" s="90" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C41" s="84" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="116" t="s">
-        <v>72</v>
-      </c>
-      <c r="E41" s="117"/>
-      <c r="F41" s="117"/>
-      <c r="H41" s="93"/>
-      <c r="I41" s="95" t="s">
-        <v>41</v>
+        <v>159</v>
+      </c>
+      <c r="D41" s="107" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="108"/>
+      <c r="F41" s="108"/>
+      <c r="H41" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I41" s="93" t="s">
+        <v>40</v>
       </c>
       <c r="J41" s="86"/>
     </row>
     <row r="42" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A42" s="82" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B42" s="90" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C42" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="D42" s="116" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="117"/>
-      <c r="F42" s="117"/>
-      <c r="H42" s="93"/>
-      <c r="I42" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J42" s="86"/>
-    </row>
-    <row r="43" spans="1:10" s="4" customFormat="1" ht="13" outlineLevel="1">
-      <c r="A43" s="113" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="114"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114"/>
-      <c r="I43" s="114"/>
-      <c r="J43" s="115"/>
+        <v>158</v>
+      </c>
+      <c r="D42" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="108"/>
+      <c r="F42" s="108"/>
+      <c r="H42" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I42" s="135" t="s">
+        <v>9</v>
+      </c>
+      <c r="J42" s="99" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A43" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="90" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="84" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" s="107" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="108"/>
+      <c r="F43" s="108"/>
+      <c r="H43" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I43" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J43" s="130"/>
     </row>
     <row r="44" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A44" s="82" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B44" s="90" t="s">
-        <v>95</v>
+        <v>194</v>
       </c>
       <c r="C44" s="84" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="116" t="s">
-        <v>58</v>
-      </c>
-      <c r="E44" s="117"/>
-      <c r="F44" s="117"/>
-      <c r="H44" s="93"/>
-      <c r="I44" s="95" t="s">
-        <v>41</v>
+        <v>157</v>
+      </c>
+      <c r="D44" s="107" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" s="108"/>
+      <c r="F44" s="108"/>
+      <c r="H44" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I44" s="93" t="s">
+        <v>40</v>
       </c>
       <c r="J44" s="86"/>
     </row>
     <row r="45" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A45" s="82" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B45" s="90" t="s">
-        <v>56</v>
+        <v>195</v>
       </c>
       <c r="C45" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="D45" s="116" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="117"/>
-      <c r="F45" s="117"/>
-      <c r="H45" s="93"/>
-      <c r="I45" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J45" s="86"/>
-    </row>
-    <row r="46" spans="1:10" s="4" customFormat="1" ht="13">
-      <c r="A46" s="113" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="114"/>
-      <c r="C46" s="114"/>
-      <c r="D46" s="114"/>
-      <c r="E46" s="114"/>
-      <c r="F46" s="114"/>
-      <c r="G46" s="114"/>
-      <c r="H46" s="114"/>
-      <c r="I46" s="114"/>
-      <c r="J46" s="115"/>
+        <v>156</v>
+      </c>
+      <c r="D45" s="107" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="108"/>
+      <c r="F45" s="108"/>
+      <c r="H45" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I45" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J45" s="99" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A46" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="90" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="84" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="E46" s="108"/>
+      <c r="F46" s="108"/>
+      <c r="H46" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I46" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46" s="130" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="47" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A47" s="82" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="B47" s="90" t="s">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="C47" s="84" t="s">
-        <v>88</v>
-      </c>
-      <c r="D47" s="116" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="117"/>
-      <c r="F47" s="117"/>
-      <c r="H47" s="93"/>
-      <c r="I47" s="95" t="s">
-        <v>41</v>
+        <v>146</v>
+      </c>
+      <c r="D47" s="107" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47" s="108"/>
+      <c r="F47" s="108"/>
+      <c r="H47" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I47" s="93" t="s">
+        <v>40</v>
       </c>
       <c r="J47" s="86"/>
     </row>
     <row r="48" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A48" s="82" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="B48" s="90" t="s">
-        <v>76</v>
+        <v>215</v>
       </c>
       <c r="C48" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48" s="116" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" s="117"/>
-      <c r="F48" s="117"/>
-      <c r="H48" s="93"/>
-      <c r="I48" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J48" s="86"/>
-    </row>
-    <row r="49" ht="12" customHeight="1"/>
-    <row r="50" ht="12" customHeight="1"/>
-    <row r="51" ht="12" customHeight="1"/>
-    <row r="52" ht="12" customHeight="1"/>
-    <row r="53" ht="12" customHeight="1"/>
-    <row r="54" ht="12" customHeight="1"/>
-    <row r="55" ht="12" customHeight="1"/>
-    <row r="56" ht="12" customHeight="1"/>
-    <row r="57" ht="12" customHeight="1"/>
-    <row r="58" ht="12" customHeight="1"/>
-    <row r="59" ht="12" customHeight="1"/>
-    <row r="60" ht="12" customHeight="1"/>
-    <row r="61" ht="12" customHeight="1"/>
-    <row r="62" ht="12" customHeight="1"/>
-    <row r="63" ht="12" customHeight="1"/>
-    <row r="64" ht="12" customHeight="1"/>
-    <row r="65" ht="12" customHeight="1"/>
-    <row r="66" ht="12" customHeight="1"/>
-    <row r="67" ht="12" customHeight="1"/>
-    <row r="68" ht="12" customHeight="1"/>
-    <row r="69" ht="12" customHeight="1"/>
-    <row r="70" ht="12" customHeight="1"/>
-    <row r="71" ht="12" customHeight="1"/>
-    <row r="72" ht="12" customHeight="1"/>
-    <row r="73" ht="12" customHeight="1"/>
-    <row r="74" ht="12" customHeight="1"/>
-    <row r="75" ht="12" customHeight="1"/>
-    <row r="76" ht="12" customHeight="1"/>
-    <row r="77" ht="12" customHeight="1"/>
-    <row r="78" ht="12" customHeight="1"/>
-    <row r="79" ht="12" customHeight="1"/>
-    <row r="80" ht="12" customHeight="1"/>
+        <v>207</v>
+      </c>
+      <c r="D48" s="107" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" s="108"/>
+      <c r="F48" s="108"/>
+      <c r="H48" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I48" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48" s="99" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A49" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="90" t="s">
+        <v>218</v>
+      </c>
+      <c r="C49" s="84" t="s">
+        <v>219</v>
+      </c>
+      <c r="D49" s="107" t="s">
+        <v>220</v>
+      </c>
+      <c r="E49" s="108"/>
+      <c r="F49" s="108"/>
+      <c r="H49" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I49" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" s="99" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A50" s="82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="107" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50" s="108"/>
+      <c r="F50" s="108"/>
+      <c r="H50" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I50" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J50" s="130" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A51" s="82" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51" s="90" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="D51" s="107" t="s">
+        <v>196</v>
+      </c>
+      <c r="E51" s="108"/>
+      <c r="F51" s="108"/>
+      <c r="H51" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I51" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J51" s="86"/>
+    </row>
+    <row r="52" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A52" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="90" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" s="107" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" s="108"/>
+      <c r="F52" s="108"/>
+      <c r="H52" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I52" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J52" s="130" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A53" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="90" t="s">
+        <v>126</v>
+      </c>
+      <c r="C53" s="84" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="107" t="s">
+        <v>223</v>
+      </c>
+      <c r="E53" s="108"/>
+      <c r="F53" s="108"/>
+      <c r="H53" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I53" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J53" s="130" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A54" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" s="90" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="84" t="s">
+        <v>149</v>
+      </c>
+      <c r="D54" s="107" t="s">
+        <v>131</v>
+      </c>
+      <c r="E54" s="108"/>
+      <c r="F54" s="108"/>
+      <c r="H54" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I54" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J54" s="79"/>
+    </row>
+    <row r="55" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A55" s="82" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="90" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="84" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" s="107" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="108"/>
+      <c r="F55" s="108"/>
+      <c r="H55" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I55" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="J55" s="79"/>
+    </row>
+    <row r="56" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A56" s="82" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="90" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" s="84" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" s="107" t="s">
+        <v>197</v>
+      </c>
+      <c r="E56" s="108"/>
+      <c r="F56" s="108"/>
+      <c r="H56" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I56" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J56" s="79" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A57" s="82" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" s="90" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="84" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" s="107" t="s">
+        <v>197</v>
+      </c>
+      <c r="E57" s="108"/>
+      <c r="F57" s="108"/>
+      <c r="H57" s="131">
+        <v>42850</v>
+      </c>
+      <c r="I57" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J57" s="79" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A58"/>
+      <c r="B58" s="91"/>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58" s="94"/>
+      <c r="J58" s="92"/>
+    </row>
+    <row r="59" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A59"/>
+      <c r="B59" s="91"/>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59" s="94"/>
+      <c r="J59" s="92"/>
+    </row>
+    <row r="60" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A60"/>
+      <c r="B60" s="91"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60" s="94"/>
+      <c r="J60" s="92"/>
+    </row>
+    <row r="61" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A61"/>
+      <c r="B61" s="91"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61" s="94"/>
+      <c r="J61" s="92"/>
+    </row>
+    <row r="62" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A62"/>
+      <c r="B62" s="91"/>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62" s="94"/>
+      <c r="J62" s="92"/>
+    </row>
+    <row r="63" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A63"/>
+      <c r="B63" s="91"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63" s="94"/>
+      <c r="J63" s="92"/>
+    </row>
+    <row r="64" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A64"/>
+      <c r="B64" s="91"/>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64" s="94"/>
+      <c r="J64" s="92"/>
+    </row>
+    <row r="65" spans="1:10" s="85" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
+      <c r="A65"/>
+      <c r="B65" s="91"/>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65" s="94"/>
+      <c r="J65" s="92"/>
+    </row>
+    <row r="66" spans="1:10" ht="12" customHeight="1"/>
+    <row r="67" spans="1:10" ht="12" customHeight="1"/>
+    <row r="68" spans="1:10" ht="12" customHeight="1"/>
+    <row r="69" spans="1:10" ht="12" customHeight="1"/>
+    <row r="70" spans="1:10" ht="12" customHeight="1"/>
+    <row r="71" spans="1:10" ht="12" customHeight="1"/>
+    <row r="72" spans="1:10" ht="12" customHeight="1"/>
+    <row r="73" spans="1:10" ht="12" customHeight="1"/>
+    <row r="74" spans="1:10" ht="12" customHeight="1"/>
+    <row r="75" spans="1:10" ht="12" customHeight="1"/>
+    <row r="76" spans="1:10" ht="12" customHeight="1"/>
+    <row r="77" spans="1:10" ht="12" customHeight="1"/>
+    <row r="78" spans="1:10" ht="12" customHeight="1"/>
+    <row r="79" spans="1:10" ht="12" customHeight="1"/>
+    <row r="80" spans="1:10" ht="12" customHeight="1"/>
     <row r="81" ht="12" customHeight="1"/>
     <row r="82" ht="12" customHeight="1"/>
     <row r="83" ht="12" customHeight="1"/>
     <row r="84" ht="12" customHeight="1"/>
     <row r="85" ht="12" customHeight="1"/>
     <row r="86" ht="12" customHeight="1"/>
+    <row r="87" ht="12" customHeight="1"/>
+    <row r="88" ht="12" customHeight="1"/>
+    <row r="89" ht="12" customHeight="1"/>
+    <row r="90" ht="12" customHeight="1"/>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="63">
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D35:F35"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D54:F54"/>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="H5:J5"/>
@@ -5534,35 +6478,32 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="I8:I9"/>
-    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:G9"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D13:F13"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D52:F52"/>
     <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="D46:F46"/>
     <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D43:F43"/>
     <mergeCell ref="D44:F44"/>
     <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
     <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D42:F42"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5581,7 +6522,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -5592,7 +6533,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23">
       <c r="A1" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="17"/>
@@ -5612,7 +6553,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -5622,9 +6563,11 @@
     </row>
     <row r="4" spans="1:7">
       <c r="B4" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="107"/>
+        <v>10</v>
+      </c>
+      <c r="C4" s="101">
+        <v>42850</v>
+      </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
@@ -5651,22 +6594,22 @@
     <row r="7" spans="1:7" ht="28">
       <c r="A7" s="20"/>
       <c r="B7" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="D7" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="55" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="55" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="64" customFormat="1">
@@ -5680,11 +6623,11 @@
       </c>
       <c r="D8" s="73">
         <f>'Manual Test Cases'!B5</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="72">
         <f>'Manual Test Cases'!B6</f>
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F8" s="72">
         <f>'Manual Test Cases'!D5</f>
@@ -5692,7 +6635,7 @@
       </c>
       <c r="G8" s="73">
         <f>'Manual Test Cases'!D6</f>
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5708,15 +6651,15 @@
       <c r="A10" s="19"/>
       <c r="B10" s="56"/>
       <c r="C10" s="57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="58">
         <f>SUM(D6:D9)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="58">
         <f>SUM(E6:E9)</f>
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F10" s="58">
         <f>SUM(F6:F9)</f>
@@ -5724,7 +6667,7 @@
       </c>
       <c r="G10" s="59">
         <f>SUM(G6:G9)</f>
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -5740,15 +6683,15 @@
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="24">
         <f>(D10+E10)*100/G10</f>
-        <v>113.04347826086956</v>
+        <v>85.106382978723403</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="25"/>
     </row>
@@ -5756,15 +6699,15 @@
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="24">
         <f>D10*100/G10</f>
-        <v>108.69565217391305</v>
+        <v>48.936170212765958</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="25"/>
     </row>

</xml_diff>